<commit_message>
Fix xlsx sheet->comments relationship
Closes python-excel/xlrd#108
</commit_message>
<xml_diff>
--- a/tests/test_comments_excel_sheet2.xlsx
+++ b/tests/test_comments_excel_sheet2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38320" windowHeight="23560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,25 +29,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="128"/>
           </rPr>
-          <t>Gunnlaugur Þór Briem:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="128"/>
-          </rPr>
-          <t xml:space="preserve">
-Note lives here</t>
+          <t>Note lives here</t>
         </r>
       </text>
     </comment>
@@ -68,7 +56,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,14 +66,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Calibri"/>

</xml_diff>